<commit_message>
New Recipes (hopefully no unusual characters)
</commit_message>
<xml_diff>
--- a/COSC345_Recipes (1).xlsx
+++ b/COSC345_Recipes (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10710"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni-my.sharepoint.com/personal/prana001_student_otago_ac_nz/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="115" documentId="8_{EFA227FA-5189-4934-925A-773C6139C4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C521C366-A944-BF4E-91C0-573A6DD6557F}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{EFA227FA-5189-4934-925A-773C6139C4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{486CC012-9929-4AB5-8C8F-B061537CFFFE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Calcifer Breakfast of eggs/bacon/cheese/bread</t>
   </si>
   <si>
-    <t>Howl’s Moving Castle</t>
-  </si>
-  <si>
     <t>Simple English breakfast</t>
   </si>
   <si>
@@ -113,18 +110,12 @@
     <t>Herring Pie or Fish Pie</t>
   </si>
   <si>
-    <t>Kiki’s Delivery Service</t>
-  </si>
-  <si>
     <t>Savoury fish pie</t>
   </si>
   <si>
     <t xml:space="preserve">4*fillets*Herring Fish, 0*null*Pastry Sheet, 1*null*Leek, 1*null*Medium White Onion, 1*null*Carrot,  5*null*Medium Potatoes, 2*cups*Spinach, 3*null*Eggs, 2*tablespoons*Mustard, 2*null*Bay Leaves, 3*cups*Milk, 2*tablespoons*Salt, 2*tablespoons*Pepper </t>
   </si>
   <si>
-    <t>1. Cut up the potatoes and put them in a pot of boiling water.  Boil for about 5 minutes, then add in two eggs and boil for 5 more minutes.  Take out the eggs, and strain the potatoes.  Then mash the potatoes in a bowl with 2/3 cup of milk./2.Add the mashed potatoes to the bottom of your casserole dish, saving about 1 potato worth of mash in the bowl./3. Slice all of the vegetables and the hardboiled eggs and saute them in a pan with some oil or butter and the bay leaves./4. Add in the rest of the milk, the mashed potato that you saved, mustard, salt and pepper.  Cook everything on medium heat stirring occasionally, until the milk reaches a thick consistency, then add it into the casserole pan.  Remember to remove the bay leaves./5. Cut the fish fillets into 3 inch wide chunks, and then add it into the casserole pan./6. Unroll the pie crust and put it on top. You can cut it into strips, and cut out a fish if you want to make it like the one in Kiki’s Delivery Service. Once you finish covering the casserole pan with the pie crust, beat an egg and brush it on top of the pie crust./7. Bake in a 350 degree oven for about 20-30 minutes, or until the crust is to your liking.</t>
-  </si>
-  <si>
     <t>Chocolate Cake</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>1*cup*Sugar,0.75*cup*Flour,0.25*cup*Cocoa Powder,1*teaspoon*Baking Soda, 0.25*teaspoon*Baking Powder, 0.25*teaspoon*Salt, 1*null*Egg, 0.5*cup*Buttermilk, 0.5*cup*Cooled Coffee, 0.25*cup*Vegetable Oil, 0.5*teaspoon*Vanilla Extract, 0.5*bag*Chocolate Chips, 0.75*cup*Heavy Whipping Cream,4*tablespoons*Salted Butter, 1*cup*White Frosting,1*null*Green Icing Pen, 1*null*Red Icing Pen</t>
   </si>
   <si>
-    <t>1. You’ll actually want to start with your frosting, since it needs extra time to chill (in fact, you can make the frosting a day ahead of time if you want). First, place your chocolate chips in a large bowl and set aside./2. Cook the whipping cream and butter in a saucepan over medium heat until just boiling, stirring frequently. Pour the cream mix over the chocolate and whisk briskly until completely smooth./3. Place some plastic wrap over the bowl and put it in the fridge to chill. After 1 hour, stir the mix thoroughly. Replace the cover and put the mix back in the fridge for another hour or until it reaches spreading consistency./4. While you’re waiting for the frosting to chill, you can bake your cake! Preheat your oven to 350°. Thoroughly spray a 9-inch round cake pan with cooking spray or grease it with butter and flour. This cake likes to stick, so be sure to thoroughly coat every nook and cranny./5. Dump the sugar, flour, cocoa, baking soda, baking powder, and salt into a large bowl. Whisk it all up!/6. Whisk in the egg, buttermilk, coffee, oil and vanilla. Beat the mix briskly for 2 minutes./7. Pour the batter into your pan and bake for 25-30 minutes or until a toothpick inserted in the center comes out clean./8. When fully baked, set the cake pan on a wire rack to cool for 10 minutes. Then flip the cake out of the pan and allow it to cool completely on the rack./9. When the cake is cool, spread on a layer of chocolate frosting. Let it set for 5-10 minutes./10. Use a toothpick to draw out where you’ll put the decorative icing. This makes it easier to replicate the look of the cake in the movie. If you make a mistake, just use an icing knife or butter knife to smooth it out./11. Pipe your decorative icing over the toothpick drawing and allow it to set for another 5-10 minutes.</t>
-  </si>
-  <si>
     <t>Bento Box</t>
   </si>
   <si>
@@ -191,9 +179,6 @@
     <t>0.25*cup*Uncooked Short Grain Rice, 250*mL*Water, 0*null*Chopped Scallion, 0*null*Umeboshi (Pickled Plums), 0*null*Toasted White Sesame Seeds, 0*null*Kizami Nori (Shredded Nori Seaweed), 0*null*Bonito Flakes (Flaked Japanese Salted Salmon), 0*null*Mitsuba (Japanese Parsley)</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Gather all the ingredients. I follow a rice-to-water ratio of 1 to 5 for a thicker consistency in this recipe; to adjust for a runnier consistency, please see the Notes at the end of the recipe card./2. Rinse ¼ cup uncooked Japanese short-grain white rice in water, then drain. Repeat until the water runs clear. Drain into a colander and shake off the excess water./3. Add the well-drained rice and 250 ml water to a heavy-bottomed pot or a donabe earthenware pot, as I have here. If cooking in a donabe, use a towel to wipe off any excess water on the bottom of the pot (or else it may crack under heat). Tip: Select a cooking pot with plenty of room for the rice and water to cook without boiling over./4. Soak the rice for at least 30 minutes./5. Cover the pot and bring to a boil over high heat./5. Once boiling, lower the heat to the stove’s lowest setting (make sure to use the right size of stove burner for your pot size). Open the lid and gently mix with a spoon, making sure the rice does not stick to the bottom of the pot./6. Then, cover with the lid and gently simmer the rice for 30 minutes. During this time, I do not open the lid or mix the rice. Tip: With a good size pot and the lowest heat on the stove, the water should not boil over. If you cook with more water or your pot is smaller than mine, you may want to leave the lid slightly ajar so the water doesn’t boil over. Tip: If you are worried, you can take a quick peek to make sure there’s enough water so the rice doesn’t burn on the bottom of the pot. If necessary, you can stir the rice or add a bit of hot water. Otherwise, don’t stir the rice because that may break the rice grains./7. After 30 minutes, turn off the heat and let it steam with the lid on for 10 minutes. The rice porridge should be soft and thick. If you want to add a beaten egg or salt, this is the time to mix it in. I keep this recipe plain and simple. Serve in individual rice bowls and garnish with toppings of your choice./8. You can keep the leftovers in an airtight container and keep them for 2 days in the refrigerator or for up to a month in the freezer. </t>
-  </si>
-  <si>
     <t>Soup Dumplings</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>Non-poisonous soup dumplings</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Heat 2 tbsp oil in pan, add mushroom and sauté till fragrant./2. Add in bamboo shoots and pork fillet. Fry till meat turn white./3. Add in seasoning and fried shallots and mix evenly. Remove from heat and set aside./4. Combine flour with water in a small mixing bowl,  stir till well dissolved./5. Bring a pot of water to a simmer. Place the bowl of flour batter over the pot. Stirring constantly and cook till batter turns thick./6. Grease 4 small bowls with corn oil. Scoop some cooked batter into each bowl. Lightly grease your fingers and press out the dough to cover the base of the bowl. Fill in meat filling. Top with another layer of cooked dough covering the fillings completely. Using greased fingers to smoothen out the edge and surface. /7. Steam the meatballs over preheated steamer over high heat for 10 minutes. Cool down for 10 minutes./8. Heat some oil in pan, remove the meatballs from the bowl and pan fry them  till lightly brown on both sides. Drain well and serve with sauce immediately./9. Optional sauce: mix and simmer 2 tablespoons sweet chilli sauce, 1 tablespoon miso paste, 4 tablespoon Hai Shan sauce, 1 tablespoon sugar, 100mL water. Add in corn starch after simmering to thicken. </t>
-  </si>
-  <si>
     <t>Steamed Buns</t>
   </si>
   <si>
@@ -218,9 +200,6 @@
     <t>60*grams*Sugar, 250*mL*Warm Water, 7*gram*Yeast, 400*grams*All Purpose Flour, 1.5*teaspoon*Baking Powder, 1*gram*Salt, 250*grams*Red Bean Paste</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Add the flour, sugar, yeast and salt into a bowl, ensuring that the salt and yeast aren’t touching. Mix thoroughly to combine. Add the water and oil, then mix with a wooden spoon until it comes together as a rough dough./ 2. Turn the dough out onto a lightly floured work surface and knead by hand (or in a stand mixer) for 10 minutes or until soft, smooth and elastic./3. Lightly coat a bowl in oil and transfer in your dough. Toss the dough in the bowl to ensure it’s fully coated in oil. Cover and allow to proof until doubled in size (about an hour)./ 4. Uncover the dough and knock out the air. Flatten the dough into a large disc and make a well in the centre. Add the baking powder into the well and gather the edges of the dough towards the centre to enclose the baking powder./5. Knead the dough for a few minutes or until the baking powder is well distributed into the dough. Flatten the dough and then divide the dough into 6 to 12 even pieces, cover any dough that isn’t being used to prevent it from drying out./6. Pat out your portioned dough into a disc and spread over a layer of red bean paste. Cup the dough in both hands and gently rotate the dough until the edges are nearly touching. Gather the edges together and twist to seal. Invert the dough so that the seam is on your work surface. Gently roll it around to help tighten that seal. Cover and rest the buns for another 20 minutes. Line your steamers and bring water to a boil in a saucepan during that time./7. Transfer the buns into a steamer lined with some baking paper, making sure to leave space between each bun as they will expand. Cover with a lid, place the steamer onto your saucepan, reduce heat to a simmer and allow to steam, undisturbed for 12 to 15 minutes (20 minutes if you want to make a massive one). Remove from heat and allow to rest for 5 minutes before opening the lid. Eat them while they’re still warm! </t>
-  </si>
-  <si>
     <t>Onigiri</t>
   </si>
   <si>
@@ -230,9 +209,6 @@
     <t>6*sheets*Roasted Seaweed (Nori), 0.75*cup*Shredded Cooked Salmon, 1*tablespoon*Mayonnaise, 6*cups*Cooked Sticky Rice, 1*null*Triangle-shaped Cookie Cutter</t>
   </si>
   <si>
-    <t>1. Start by slicing your nori sheets in half lengthwise. My sheets were 2 ½” x 3 ½”, so in the end I had 12 strips that were 1 ¼” wide. Mix the mayonnaise into your salmon until well coated. Set the salmon mix and nori aside./2. Put the cookie cutter on a flat surface. Place an 8″x8″ sheet of plastic wrap over the cookie cutter and push some of it it down inside so that the inside of the cookie cutter is completely lined with plastic wrap. Scoop approximately 2 tbsp of rice into the bottom of the cutter and press it flat with a plastic spoon or small rubber spatula (the rice won’t stick to the tools as much as it sticks to fingers!). When flattening the rice, push it around so that it reaches right up to the corners of the cutter (add more rice if needed to make sure the bottom is completely coated). Place 1 tsp salmon filling into the middle of the rice, spreading it around just a little, so there will be a little salmon in each bite of rice when you’re finished./3. Place a couple more tablespoons of rice on top and flatten out as before. Add a little extra rice if you need more to cover up the salmon. Wrap the plastic tightly over the exposed end of the onigiri and pop it out of the cookie cutter. Firmly wrap any loose ends around the outside of the onigiri. Set aside. /4. Repeat with remaining rice and salmon until you run out of ingredients (for me, this made 12 rice balls)./5. Let the onigiri set for 5-10 minutes. If planning to eat them later, place them on a baking sheet and chill until ready to serve (you can reheat them in the microwave inside the plastic wrap for no more than 20-25 seconds—if they get too hot, they can fall apart). /6. When ready to serve, remove the plastic wrap and press a nori strip around the bottom of each onigiri. The rice should still be sticky enough that the nori adheres with no problems.</t>
-  </si>
-  <si>
     <t>Vanilla Chiffon Cake</t>
   </si>
   <si>
@@ -269,9 +245,6 @@
     <t>4*null*Horse Mackerel Fish, 0.25*teaspoon*Salt, 0.25*teaspoon*Pepper, 1.5*tablespoon*Flour, 1*null*Egg (Beaten), 1.5*cups*Panko Breadcrumbs, 0*null*Oil for Frying, 0*null*Shredded Lettuce, 0*null*Tonkatsu Sauce</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Remove the scales on both sides of the fish by sliding the tip of the knife from the tail end towards the head./2. 	1	Place the knife where the tail begins, facing the blade to the head. Move the knife at a very low angle towards the head and trim the bony scales (scutes) along the lateral line, which ends close to half-way./3. Remove the head by cutting at a slight angle behind the gill and the front fin./4. Using a finger or a narrow knife, remove the guts from the opening, without breaking the thin flesh around the belly./5. Rinse the fish and clean the cavity in the belly. Pat dry, including inside the cavity. /6. Starting from the head of the fish, make a shallow incision on the dorsal side all the way to the tail. The incision needs to be on your side of the back bones./7. Using the tip of the knife, extend the incision towards the belly along the backbones. It is easier if you lift the flesh that is already removed from the bones so that you can see where your knife is cutting./8. Detach the rib cage by cutting the rib bones along the back bones./9. Continue to remove the flesh along the back bones until you reach to the belly, but keep the belly skin intact. You now have a butterflied fish with the bone in./10. Flip the butterflied fish over (skin side up) and make an incision on the other side of the dorsal in the same way./11. Chop the backbone at the tail end, keeping the tail attached to the flesh./12. Now you have a butterflied fish fillet. If small pieces of guts are left on the belly, wipe them off using kitchen paper./13. Place the tip of the knife where the rib bones start and trim the flesh with the rib bones very thinly. Do the same on the other side of the rib bones./14. There is a very sharp hard thorn in front of the anal fin. You need to remove it. I used kitchen scissors for this./15. The last step is to remove the pin bones from the fillet. Run your finger along where the backbone was and feel the bones to locate them. Remove all of them using a pair of fish bone tweezers or pliers./16. Sprinkle salt and pepper over both sides of butterflied fish fillets./17. Working one fillet at a time, coat a fillet with flour, then pat to shake off excess flour. Place it in the egg and coat all over. Allow excess egg to drip, then transfer to the breadcrumbs./18. Cover the entire fish with breadcrumbs, and gently press down so that a good layer of breadcrumbs is stuck on both sides. Repeat for the rest of the fillets./19. Heat oil in a frying pan to 170°C / 338°F. The oil should be about 3cm / 1¼” deep./20. Gently place the crumbed fish skin side up. Do not crowd the oil with too many fish pieces. Cook for about 1-1½ minutes, then turn the fish over. Cook for further 1 minutes or so, until golden brown./21. Transfer the fried fish to a tray lined with kitchen paper to drain excess oil./22. Place two Aji Fry pieces with shredded lettuce on each serving plate. Serve immediately with the sauce of your choice. </t>
-  </si>
-  <si>
     <t>Hard</t>
   </si>
   <si>
@@ -357,6 +330,33 @@
   </si>
   <si>
     <t xml:space="preserve">1. Chop the carrots, broccoli, cauliflower, and potatoes into small pieces./2. Slice the leek into thin slices./3. Mince the garlic./4. Heat olive oil on medium heat and cook the sliced leeks till it has softened./5. Add about 5 cups of water and 1 tsp of salt./6. When the water has reached a boil, add all of the chopped vegetables. Make sure that the vegetables are fully submerged in water. /7. Boil for less than 5 minutes. Pierce with a fork to see if the vegetables are soft enough./8. Remove the vegetables from the pot and set it aside. /9. With the remaining water left in the pot, add flour and milk. Whisk until it reaches a thick consistency./10. Boil the mixture while whisking. Add the boiled vegetables and season it with salt and pepper./11. Transfer it to a bowl and garnish with parsley. </t>
+  </si>
+  <si>
+    <t>Howl's Moving Castle</t>
+  </si>
+  <si>
+    <t>Kiki's Delivery Service</t>
+  </si>
+  <si>
+    <t>1. Cut up the potatoes and put them in a pot of boiling water.  Boil for about 5 minutes, then add in two eggs and boil for 5 more minutes.  Take out the eggs, and strain the potatoes.  Then mash the potatoes in a bowl with 2/3 cup of milk./2.Add the mashed potatoes to the bottom of your casserole dish, saving about 1 potato worth of mash in the bowl./3. Slice all of the vegetables and the hardboiled eggs and saute them in a pan with some oil or butter and the bay leaves./4. Add in the rest of the milk, the mashed potato that you saved, mustard, salt and pepper.  Cook everything on medium heat stirring occasionally, until the milk reaches a thick consistency, then add it into the casserole pan.  Remember to remove the bay leaves./5. Cut the fish fillets into 3 inch wide chunks, and then add it into the casserole pan./6. Unroll the pie crust and put it on top. You can cut it into strips, and cut out a fish if you want to make it like the one in Kiki's Delivery Service. Once you finish covering the casserole pan with the pie crust, beat an egg and brush it on top of the pie crust./7. Bake in a 350 degree oven for about 20-30 minutes, or until the crust is to your liking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Gather all the ingredients. I follow a rice-to-water ratio of 1 to 5 for a thicker consistency in this recipe; to adjust for a runnier consistency, please see the Notes at the end of the recipe card./2. Rinse ¼ cup uncooked Japanese short-grain white rice in water, then drain. Repeat until the water runs clear. Drain into a colander and shake off the excess water./3. Add the well-drained rice and 250 ml water to a heavy-bottomed pot or a donabe earthenware pot, as I have here. If cooking in a donabe, use a towel to wipe off any excess water on the bottom of the pot (or else it may crack under heat). Tip: Select a cooking pot with plenty of room for the rice and water to cook without boiling over./4. Soak the rice for at least 30 minutes./5. Cover the pot and bring to a boil over high heat./5. Once boiling, lower the heat to the stove's lowest setting (make sure to use the right size of stove burner for your pot size). Open the lid and gently mix with a spoon, making sure the rice does not stick to the bottom of the pot./6. Then, cover with the lid and gently simmer the rice for 30 minutes. During this time, I do not open the lid or mix the rice. Tip: With a good size pot and the lowest heat on the stove, the water should not boil over. If you cook with more water or your pot is smaller than mine, you may want to leave the lid slightly ajar so the water doesn't boil over. Tip: If you are worried, you can take a quick peek to make sure there's enough water so the rice doesn't burn on the bottom of the pot. If necessary, you can stir the rice or add a bit of hot water. Otherwise, don't stir the rice because that may break the rice grains./7. After 30 minutes, turn off the heat and let it steam with the lid on for 10 minutes. The rice porridge should be soft and thick. If you want to add a beaten egg or salt, this is the time to mix it in. I keep this recipe plain and simple. Serve in individual rice bowls and garnish with toppings of your choice./8. You can keep the leftovers in an airtight container and keep them for 2 days in the refrigerator or for up to a month in the freezer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add the flour, sugar, yeast and salt into a bowl, ensuring that the salt and yeast aren't touching. Mix thoroughly to combine. Add the water and oil, then mix with a wooden spoon until it comes together as a rough dough./ 2. Turn the dough out onto a lightly floured work surface and knead by hand (or in a stand mixer) for 10 minutes or until soft, smooth and elastic./3. Lightly coat a bowl in oil and transfer in your dough. Toss the dough in the bowl to ensure it's fully coated in oil. Cover and allow to proof until doubled in size (about an hour)./ 4. Uncover the dough and knock out the air. Flatten the dough into a large disc and make a well in the centre. Add the baking powder into the well and gather the edges of the dough towards the centre to enclose the baking powder./5. Knead the dough for a few minutes or until the baking powder is well distributed into the dough. Flatten the dough and then divide the dough into 6 to 12 even pieces, cover any dough that isn't being used to prevent it from drying out./6. Pat out your portioned dough into a disc and spread over a layer of red bean paste. Cup the dough in both hands and gently rotate the dough until the edges are nearly touching. Gather the edges together and twist to seal. Invert the dough so that the seam is on your work surface. Gently roll it around to help tighten that seal. Cover and rest the buns for another 20 minutes. Line your steamers and bring water to a boil in a saucepan during that time./7. Transfer the buns into a steamer lined with some baking paper, making sure to leave space between each bun as they will expand. Cover with a lid, place the steamer onto your saucepan, reduce heat to a simmer and allow to steam, undisturbed for 12 to 15 minutes (20 minutes if you want to make a massive one). Remove from heat and allow to rest for 5 minutes before opening the lid. Eat them while they're still warm! </t>
+  </si>
+  <si>
+    <t>1. Start by slicing your nori sheets in half lengthwise. My sheets were 2.5” x 3.5”, so in the end I had 12 strips that were 1.25” wide. Mix the mayonnaise into your salmon until well coated. Set the salmon mix and nori aside./2. Put the cookie cutter on a flat surface. Place an 8″x8″ sheet of plastic wrap over the cookie cutter and push some of it it down inside so that the inside of the cookie cutter is completely lined with plastic wrap. Scoop approximately 2 tbsp of rice into the bottom of the cutter and press it flat with a plastic spoon or small rubber spatula (the rice won't stick to the tools as much as it sticks to fingers!). When flattening the rice, push it around so that it reaches right up to the corners of the cutter (add more rice if needed to make sure the bottom is completely coated). Place 1 tsp salmon filling into the middle of the rice, spreading it around just a little, so there will be a little salmon in each bite of rice when you're finished./3. Place a couple more tablespoons of rice on top and flatten out as before. Add a little extra rice if you need more to cover up the salmon. Wrap the plastic tightly over the exposed end of the onigiri and pop it out of the cookie cutter. Firmly wrap any loose ends around the outside of the onigiri. Set aside. /4. Repeat with remaining rice and salmon until you run out of ingredients (for me, this made 12 rice balls)./5. Let the onigiri set for 5-10 minutes. If planning to eat them later, place them on a baking sheet and chill until ready to serve (you can reheat them in the microwave inside the plastic wrap for no more than 20-25 seconds—if they get too hot, they can fall apart). /6. When ready to serve, remove the plastic wrap and press a nori strip around the bottom of each onigiri. The rice should still be sticky enough that the nori adheres with no problems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Heat 2 tbsp oil in pan, add mushroom and saute till fragrant./2. Add in bamboo shoots and pork fillet. Fry till meat turn white./3. Add in seasoning and fried shallots and mix evenly. Remove from heat and set aside./4. Combine flour with water in a small mixing bowl,  stir till well dissolved./5. Bring a pot of water to a simmer. Place the bowl of flour batter over the pot. Stirring constantly and cook till batter turns thick./6. Grease 4 small bowls with corn oil. Scoop some cooked batter into each bowl. Lightly grease your fingers and press out the dough to cover the base of the bowl. Fill in meat filling. Top with another layer of cooked dough covering the fillings completely. Using greased fingers to smoothen out the edge and surface. /7. Steam the meatballs over preheated steamer over high heat for 10 minutes. Cool down for 10 minutes./8. Heat some oil in pan, remove the meatballs from the bowl and pan fry them  till lightly brown on both sides. Drain well and serve with sauce immediately./9. Optional sauce: mix and simmer 2 tablespoons sweet chilli sauce, 1 tablespoon miso paste, 4 tablespoon Hai Shan sauce, 1 tablespoon sugar, 100mL water. Add in corn starch after simmering to thicken. </t>
+  </si>
+  <si>
+    <t>1. You'll actually want to start with your frosting, since it needs extra time to chill (in fact, you can make the frosting a day ahead of time if you want). First, place your chocolate chips in a large bowl and set aside./2. Cook the whipping cream and butter in a saucepan over medium heat until just boiling, stirring frequently. Pour the cream mix over the chocolate and whisk briskly until completely smooth./3. Place some plastic wrap over the bowl and put it in the fridge to chill. After 1 hour, stir the mix thoroughly. Replace the cover and put the mix back in the fridge for another hour or until it reaches spreading consistency./4. While you're waiting for the frosting to chill, you can bake your cake! Preheat your oven to 350 degrees. Thoroughly spray a 9-inch round cake pan with cooking spray or grease it with butter and flour. This cake likes to stick, so be sure to thoroughly coat every nook and cranny./5. Dump the sugar, flour, cocoa, baking soda, baking powder, and salt into a large bowl. Whisk it all up!/6. Whisk in the egg, buttermilk, coffee, oil and vanilla. Beat the mix briskly for 2 minutes./7. Pour the batter into your pan and bake for 25-30 minutes or until a toothpick inserted in the center comes out clean./8. When fully baked, set the cake pan on a wire rack to cool for 10 minutes. Then flip the cake out of the pan and allow it to cool completely on the rack./9. When the cake is cool, spread on a layer of chocolate frosting. Let it set for 5-10 minutes./10. Use a toothpick to draw out where you'll put the decorative icing. This makes it easier to replicate the look of the cake in the movie. If you make a mistake, just use an icing knife or butter knife to smooth it out./11. Pipe your decorative icing over the toothpick drawing and allow it to set for another 5-10 minutes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Remove the scales on both sides of the fish by sliding the tip of the knife from the tail end towards the head./2. Place the knife where the tail begins, facing the blade to the head. Move the knife at a very low angle towards the head and trim the bony scales (scutes) along the lateral line, which ends close to half-way./3. Remove the head by cutting at a slight angle behind the gill and the front fin./4. Using a finger or a narrow knife, remove the guts from the opening, without breaking the thin flesh around the belly./5. Rinse the fish and clean the cavity in the belly. Pat dry, including inside the cavity. /6. Starting from the head of the fish, make a shallow incision on the dorsal side all the way to the tail. The incision needs to be on your side of the back bones./7. Using the tip of the knife, extend the incision towards the belly along the backbones. It is easier if you lift the flesh that is already removed from the bones so that you can see where your knife is cutting./8. Detach the rib cage by cutting the rib bones along the back bones./9. Continue to remove the flesh along the back bones until you reach to the belly, but keep the belly skin intact. You now have a butterflied fish with the bone in./10. Flip the butterflied fish over (skin side up) and make an incision on the other side of the dorsal in the same way./11. Chop the backbone at the tail end, keeping the tail attached to the flesh./12. Now you have a butterflied fish fillet. If small pieces of guts are left on the belly, wipe them off using kitchen paper./13. Place the tip of the knife where the rib bones start and trim the flesh with the rib bones very thinly. Do the same on the other side of the rib bones./14. There is a very sharp hard thorn in front of the anal fin. You need to remove it. I used kitchen scissors for this./15. The last step is to remove the pin bones from the fillet. Run your finger along where the backbone was and feel the bones to locate them. Remove all of them using a pair of fish bone tweezers or pliers./16. Sprinkle salt and pepper over both sides of butterflied fish fillets./17. Working one fillet at a time, coat a fillet with flour, then pat to shake off excess flour. Place it in the egg and coat all over. Allow excess egg to drip, then transfer to the breadcrumbs./18. Cover the entire fish with breadcrumbs, and gently press down so that a good layer of breadcrumbs is stuck on both sides. Repeat for the rest of the fillets./19. Heat oil in a frying pan to 170 degrees C / 338 degrees F. The oil should be about 3cm / 1.25” deep./20. Gently place the crumbed fish skin side up. Do not crowd the oil with too many fish pieces. Cook for about 1-1.5 minutes, then turn the fish over. Cook for further 1 minutes or so, until golden brown./21. Transfer the fried fish to a tray lined with kitchen paper to drain excess oil./22. Place two Aji Fry pieces with shredded lettuce on each serving plate. Serve immediately with the sauce of your choice. </t>
   </si>
 </sst>
 </file>
@@ -410,21 +410,23 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,533 +765,534 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="C11" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.16015625" customWidth="1"/>
-    <col min="2" max="2" width="21.1171875" customWidth="1"/>
-    <col min="3" max="3" width="22.1953125" customWidth="1"/>
-    <col min="4" max="4" width="79.50390625" customWidth="1"/>
-    <col min="5" max="5" width="74.390625" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="79.54296875" customWidth="1"/>
+    <col min="5" max="5" width="74.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>720</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="4">
+        <v>40</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="4">
+        <v>150</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="4">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="4">
+        <v>720</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
+        <v>40</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="4">
+        <v>65</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="4">
         <v>40</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="4">
+        <v>120</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="4">
+        <v>15</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="4">
+        <v>150</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="4">
+        <v>150</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="4">
+        <v>50</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="4">
+        <v>15</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="4">
+        <v>40</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="4">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <v>150</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7">
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="4">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="4">
+        <v>20</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="4">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8">
-        <v>720</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9">
-        <v>40</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="G22" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10">
-        <v>65</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11">
-        <v>40</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12">
-        <v>120</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13">
-        <v>15</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14">
-        <v>150</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15">
-        <v>150</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
-      <c r="G16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="121.5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18">
-        <v>40</v>
-      </c>
-      <c r="G18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="121.5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22">
-        <v>30</v>
-      </c>
-      <c r="G22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C26" s="4"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding instructions for spaghetti bolognese
</commit_message>
<xml_diff>
--- a/COSC345_Recipes (1).xlsx
+++ b/COSC345_Recipes (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natas\Downloads\COSC345\Realm-of-Feasts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadia\Downloads\UNI-work\COSC345\Realm-of-Feasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942C0E9-A2B1-4F74-B2E1-285D53CB5256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAFF85F-B94F-4779-8204-BAC7B91AE5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D48BFF6E-7DE3-47B5-ADE0-6EAA34E0C134}"/>
   </bookViews>
   <sheets>
     <sheet name="COSC345_Recipes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t xml:space="preserve">53*grams*Vegetable Oil, 3*null*Eggs, 90*mL*Water, 1*tablespoon*Vanilla Extract, 140*grams*Cake Flour, 268*grams*Granulated White Sugar, 0.5*tablespoon*Baking Powder, 0.25*teaspoon*Salt, 0.5*teaspoon*Cream of Tartar, 90*grams*Egg Whites (Room temp), 225*grams*Unsalted Butter (Room temp &amp; cubed), 0.5*teaspoon*lemon juice, 1*teaspoon*Lemon Zest, 0*null*Yellow Food Colouring </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Heat up the oil and add the onions. Cook in med low until they are slightly soft and slightly see through not all the way. about 3-5 mins./2. Add the garlic and cook on low for another 3 minuets till everything is soft and slightly colored. Don't cook it till it’s brown then it’ll be burnt and wont taste good./3. Open the can of crushed tomatoes and add it. Cook on med low for about 10 mins./4. Add the bay leafs, Italian spices, salt, and pepper and if you have some fresh basil stir everything and let it cook for another 10-15 minuets. Now if you arent sure about how much spices you want I would add a little bit and add more if you feel like you need it. It is easier to add then to take away and you dont want the sauce to be ruined by over seasoning it./5. After the sauces has been cooking I like to taste it at this point and see how it tastes. Then I’ll add the sugar again same thing add a little and taste till it’s perfect for you. I then cook for another 5 minutes and then turn the heat off and let it stand./6. As the sauce is standing I start the pasta. Just put a pot of water on the stove and wait for it to boil.Once it’s boiling I add a little salt and oil this keeps the pasta from sticking and gives it a little bit of a taste./7. I like my pasta al dente so I check after 9-10 minuets to see if it’s ready if you like it softer then wait longer./8. Strain the pasta heat up the sauce quickly if it’s cooled too much and it’s done!/9. </t>
   </si>
 </sst>
 </file>
@@ -410,23 +413,23 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -765,50 +768,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E378D-9781-4302-9477-07B2B463A36A}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="79.5546875" customWidth="1"/>
-    <col min="5" max="5" width="74.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="79.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="74.36328125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -817,21 +821,21 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -840,21 +844,21 @@
       <c r="E3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>720</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -863,67 +867,67 @@
       <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>5</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>40</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>150</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -932,18 +936,18 @@
       <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>30</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -955,18 +959,18 @@
       <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>720</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" ht="232" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -975,19 +979,21 @@
       <c r="D9" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4">
+      <c r="E9" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="1">
         <v>40</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -996,21 +1002,21 @@
       <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>65</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1019,21 +1025,21 @@
       <c r="D11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>40</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1042,257 +1048,257 @@
       <c r="D12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>120</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="1">
         <v>15</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:7" ht="348" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="1">
         <v>150</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:7" ht="203" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="1">
         <v>150</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="1">
         <v>50</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="1">
         <v>15</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:7" ht="319" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="1">
         <v>40</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="1">
         <v>30</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:7" ht="145" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="1">
         <v>20</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="1">
         <v>30</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="2"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>